<commit_message>
add multi-task learning for LM model
</commit_message>
<xml_diff>
--- a/plots.xlsx
+++ b/plots.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="32720" windowHeight="20320" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="L1 Pair" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>GRU L1 Pair epoch=40, epoch_pred = 2</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -94,6 +94,15 @@
   <si>
     <t xml:space="preserve"> test loss</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Train loss</t>
+  </si>
+  <si>
+    <t>Eval loss</t>
+  </si>
+  <si>
+    <t>Epoch</t>
   </si>
 </sst>
 </file>
@@ -175,7 +184,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -367,11 +375,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1610022256"/>
-        <c:axId val="-1610020208"/>
+        <c:axId val="-2122859568"/>
+        <c:axId val="-2122857520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1610022256"/>
+        <c:axId val="-2122859568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -428,12 +436,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1610020208"/>
+        <c:crossAx val="-2122857520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1610020208"/>
+        <c:axId val="-2122857520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -490,7 +498,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1610022256"/>
+        <c:crossAx val="-2122859568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -746,11 +754,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1652171488"/>
-        <c:axId val="-1652169440"/>
+        <c:axId val="-2130030464"/>
+        <c:axId val="-2130027984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1652171488"/>
+        <c:axId val="-2130030464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -807,12 +815,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1652169440"/>
+        <c:crossAx val="-2130027984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1652169440"/>
+        <c:axId val="-2130027984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -869,7 +877,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1652171488"/>
+        <c:crossAx val="-2130030464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1278,11 +1286,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1686647296"/>
-        <c:axId val="-1686645232"/>
+        <c:axId val="-2130003376"/>
+        <c:axId val="-2130000896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1686647296"/>
+        <c:axId val="-2130003376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1339,12 +1347,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1686645232"/>
+        <c:crossAx val="-2130000896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1686645232"/>
+        <c:axId val="-2130000896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1401,7 +1409,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1686647296"/>
+        <c:crossAx val="-2130003376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1689,11 +1697,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1686613680"/>
-        <c:axId val="-1686611200"/>
+        <c:axId val="-2122736944"/>
+        <c:axId val="-2122720208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1686613680"/>
+        <c:axId val="-2122736944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1750,12 +1758,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1686611200"/>
+        <c:crossAx val="-2122720208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1686611200"/>
+        <c:axId val="-2122720208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1812,7 +1820,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1686613680"/>
+        <c:crossAx val="-2122736944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2233,11 +2241,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1686586496"/>
-        <c:axId val="-1686584016"/>
+        <c:axId val="-2122690384"/>
+        <c:axId val="-2122687904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1686586496"/>
+        <c:axId val="-2122690384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2294,12 +2302,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1686584016"/>
+        <c:crossAx val="-2122687904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1686584016"/>
+        <c:axId val="-2122687904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2356,7 +2364,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1686586496"/>
+        <c:crossAx val="-2122690384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2370,7 +2378,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.848996062992126"/>
+          <c:y val="0.583247912192794"/>
+          <c:w val="0.131003937007874"/>
+          <c:h val="0.183031448341685"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2521,6 +2538,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'LM one-hot'!$B$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Train loss</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="31750" cap="rnd">
               <a:noFill/>
@@ -2626,6 +2654,17 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'LM one-hot'!$C$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Eval loss</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="31750" cap="rnd">
               <a:noFill/>
@@ -2736,11 +2775,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1651796480"/>
-        <c:axId val="-1651763936"/>
+        <c:axId val="-2069854976"/>
+        <c:axId val="-2094334608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1651796480"/>
+        <c:axId val="-2069854976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2796,12 +2835,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1651763936"/>
+        <c:crossAx val="-2094334608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1651763936"/>
+        <c:axId val="-2094334608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2857,7 +2896,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1651796480"/>
+        <c:crossAx val="-2069854976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2978,7 +3017,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3298,11 +3336,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1688011488"/>
-        <c:axId val="-1688026304"/>
+        <c:axId val="-2122832608"/>
+        <c:axId val="-2122829856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1688011488"/>
+        <c:axId val="-2122832608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3359,12 +3397,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1688026304"/>
+        <c:crossAx val="-2122829856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1688026304"/>
+        <c:axId val="-2122829856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3421,7 +3459,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1688011488"/>
+        <c:crossAx val="-2122832608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3435,7 +3473,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3542,7 +3579,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3724,11 +3760,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1652227184"/>
-        <c:axId val="-1652224704"/>
+        <c:axId val="-2122809680"/>
+        <c:axId val="-2122807200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1652227184"/>
+        <c:axId val="-2122809680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3785,12 +3821,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1652224704"/>
+        <c:crossAx val="-2122807200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1652224704"/>
+        <c:axId val="-2122807200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3847,7 +3883,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1652227184"/>
+        <c:crossAx val="-2122809680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3911,7 +3947,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4103,11 +4138,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1686736896"/>
-        <c:axId val="-1686734416"/>
+        <c:axId val="-2122776768"/>
+        <c:axId val="-2122774288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1686736896"/>
+        <c:axId val="-2122776768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4164,12 +4199,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1686734416"/>
+        <c:crossAx val="-2122774288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1686734416"/>
+        <c:axId val="-2122774288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4226,7 +4261,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1686736896"/>
+        <c:crossAx val="-2122776768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4315,7 +4350,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4635,11 +4669,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1686709616"/>
-        <c:axId val="-1686707136"/>
+        <c:axId val="-2122747520"/>
+        <c:axId val="-2122745456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1686709616"/>
+        <c:axId val="-2122747520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4696,12 +4730,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1686707136"/>
+        <c:crossAx val="-2122745456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1686707136"/>
+        <c:axId val="-2122745456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4758,7 +4792,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1686709616"/>
+        <c:crossAx val="-2122747520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4772,7 +4806,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4879,7 +4912,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5061,11 +5093,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1609992736"/>
-        <c:axId val="-1609990256"/>
+        <c:axId val="-2122727712"/>
+        <c:axId val="-2122725232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1609992736"/>
+        <c:axId val="-2122727712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5122,12 +5154,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1609990256"/>
+        <c:crossAx val="-2122725232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1609990256"/>
+        <c:axId val="-2122725232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5184,7 +5216,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1609992736"/>
+        <c:crossAx val="-2122727712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5248,7 +5280,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5440,11 +5471,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1652189200"/>
-        <c:axId val="-1652186720"/>
+        <c:axId val="-2130111136"/>
+        <c:axId val="-2130109072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1652189200"/>
+        <c:axId val="-2130111136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5501,12 +5532,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1652186720"/>
+        <c:crossAx val="-2130109072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1652186720"/>
+        <c:axId val="-2130109072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5563,7 +5594,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1652189200"/>
+        <c:crossAx val="-2130111136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5652,7 +5683,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5972,11 +6002,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1686723840"/>
-        <c:axId val="-1686722480"/>
+        <c:axId val="-2130081872"/>
+        <c:axId val="-2130079392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1686723840"/>
+        <c:axId val="-2130081872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6033,12 +6063,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1686722480"/>
+        <c:crossAx val="-2130079392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1686722480"/>
+        <c:axId val="-2130079392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6095,7 +6125,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1686723840"/>
+        <c:crossAx val="-2130081872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6109,7 +6139,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6216,7 +6245,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6398,11 +6426,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1686677872"/>
-        <c:axId val="-1686675392"/>
+        <c:axId val="-2130059216"/>
+        <c:axId val="-2130056736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1686677872"/>
+        <c:axId val="-2130059216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6459,12 +6487,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1686675392"/>
+        <c:crossAx val="-2130056736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1686675392"/>
+        <c:axId val="-2130056736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6521,7 +6549,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1686677872"/>
+        <c:crossAx val="-2130059216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14788,20 +14816,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="6" name="Chart 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -15967,8 +15995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16213,8 +16241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="T55" sqref="T55"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16446,6 +16474,17 @@
       </c>
       <c r="D17">
         <v>2.6387393474600001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>